<commit_message>
Likert Scale implementation for remaining courses
</commit_message>
<xml_diff>
--- a/src/ACAT/assessment_results/COMP-103_FA24_01_outcomes.xlsx
+++ b/src/ACAT/assessment_results/COMP-103_FA24_01_outcomes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,30 +436,35 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Understand and implement advanced programming concepts building upon the foundational knowledge acquired in Programming I.</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Implement functional abstraction and recursion in solving computational problems.</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Apply basic software engineering practices such as version control, debugging, and testing frameworks.</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Write efficient, readable, and well-documented complex code.</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Work effectively in a collaborative environment to develop moderately complex software solutions.</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Apply programming skills to solve real-world problems and develop software solutions.</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Understand global issues and cultural diversity in computing.</t>
         </is>
@@ -475,7 +480,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
         <v>5</v>
@@ -487,6 +492,9 @@
         <v>5</v>
       </c>
       <c r="G2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" t="n">
         <v>4</v>
       </c>
     </row>
@@ -500,7 +508,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
         <v>4</v>
@@ -512,6 +520,9 @@
         <v>4</v>
       </c>
       <c r="G3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3" t="n">
         <v>5</v>
       </c>
     </row>
@@ -537,6 +548,9 @@
         <v>4</v>
       </c>
       <c r="G4" t="n">
+        <v>4</v>
+      </c>
+      <c r="H4" t="n">
         <v>5</v>
       </c>
     </row>
@@ -550,7 +564,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
         <v>5</v>
@@ -562,6 +576,9 @@
         <v>5</v>
       </c>
       <c r="G5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" t="n">
         <v>4</v>
       </c>
     </row>
@@ -575,7 +592,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
         <v>5</v>
@@ -587,6 +604,9 @@
         <v>5</v>
       </c>
       <c r="G6" t="n">
+        <v>5</v>
+      </c>
+      <c r="H6" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dropped NaN's from grade excel
</commit_message>
<xml_diff>
--- a/src/ACAT/assessment_results/COMP-103_FA24_01_outcomes.xlsx
+++ b/src/ACAT/assessment_results/COMP-103_FA24_01_outcomes.xlsx
@@ -471,10 +471,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Student_1      </t>
-        </is>
+      <c r="A2" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="B2" t="n">
         <v>4</v>
@@ -499,10 +497,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Student_2      </t>
-        </is>
+      <c r="A3" s="1" t="n">
+        <v>12</v>
       </c>
       <c r="B3" t="n">
         <v>5</v>
@@ -527,10 +523,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Student_3      </t>
-        </is>
+      <c r="A4" s="1" t="n">
+        <v>13</v>
       </c>
       <c r="B4" t="n">
         <v>4</v>
@@ -555,10 +549,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Student_4      </t>
-        </is>
+      <c r="A5" s="1" t="n">
+        <v>14</v>
       </c>
       <c r="B5" t="n">
         <v>4</v>
@@ -583,10 +575,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Student_5      </t>
-        </is>
+      <c r="A6" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="B6" t="n">
         <v>4</v>

</xml_diff>